<commit_message>
[IMP] Adjust CD Receivable Balance Sheet Detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_detail.xlsx
@@ -255,6 +255,21 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF685"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -292,7 +307,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFF685"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -325,7 +340,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -475,6 +490,16 @@
       <c r="AMJ13" s="0"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:L1048576">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Subtotal",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:L1048576">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Grand Total",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>